<commit_message>
Updated drawings & description to match Ponoko uploader
Updated drawings & description to match Ponoko uploader
</commit_message>
<xml_diff>
--- a/docs/build_instructions_standard.xlsx
+++ b/docs/build_instructions_standard.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="445" documentId="415E32CF7F9D79DA378485C62B6EEDB6DC1C7F04" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3FC29E3D-8C47-45A0-8B96-DBA66387DCD9}"/>
+  <xr:revisionPtr revIDLastSave="448" documentId="415E32CF7F9D79DA378485C62B6EEDB6DC1C7F04" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F5FB1701-8FBD-4EF4-AC23-85DD750CED2A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -642,7 +642,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>